<commit_message>
feat: Loading report to excel and creating excel file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -64,8 +64,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,108 +398,346 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="48.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Serial Number</v>
+        <v>assetid</v>
       </c>
       <c r="B1" t="str">
-        <v>Acquisition Date</v>
+        <v>serialnumber</v>
       </c>
       <c r="C1" t="str">
-        <v>Condition</v>
+        <v>acquisitiondate</v>
       </c>
       <c r="D1" t="str">
-        <v>Responsible User's Name</v>
+        <v>condition</v>
       </c>
       <c r="E1" t="str">
-        <v>Acquisition Cost</v>
+        <v>acquisitioncost</v>
       </c>
       <c r="F1" t="str">
-        <v>Residual Value</v>
+        <v>residualvalue</v>
       </c>
       <c r="G1" t="str">
-        <v>Category Name</v>
+        <v>usefullife</v>
       </c>
       <c r="H1" t="str">
-        <v>Useful Life</v>
+        <v>barcode</v>
       </c>
       <c r="I1" t="str">
-        <v>Barcode</v>
+        <v>description</v>
       </c>
       <c r="J1" t="str">
-        <v>Description</v>
+        <v>disposaldate</v>
       </c>
       <c r="K1" t="str">
-        <v>Expected Depreciation Date</v>
+        <v>isconverted</v>
       </c>
       <c r="L1" t="str">
-        <v>Days To Disposal</v>
+        <v>category</v>
       </c>
       <c r="M1" t="str">
-        <v>Site</v>
+        <v>location_name</v>
       </c>
       <c r="N1" t="str">
-        <v>Building</v>
+        <v>depreciationtype</v>
       </c>
       <c r="O1" t="str">
-        <v>Office</v>
+        <v>responsible_user</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
-        <v>ISBN 0023423423</v>
+      <c r="A2">
+        <v>5</v>
       </c>
       <c r="B2" t="str">
-        <v>2024-12-12</v>
-      </c>
-      <c r="C2" t="str">
+        <v>ISBN 987-897231232</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45058.000185185185</v>
+      </c>
+      <c r="D2" t="str">
         <v>Good</v>
       </c>
-      <c r="D2" t="str">
-        <v>Benoit Blanc</v>
-      </c>
       <c r="E2">
+        <v>10000</v>
+      </c>
+      <c r="F2">
         <v>1000</v>
       </c>
-      <c r="G2" t="str">
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2" t="str">
+        <v>AUA1000</v>
+      </c>
+      <c r="I2" t="str">
+        <v>This would have been an epic description but nah</v>
+      </c>
+      <c r="J2" s="1">
+        <v>45150.000185185185</v>
+      </c>
+      <c r="K2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" t="str">
         <v>NewCategory</v>
       </c>
-      <c r="H2">
+      <c r="M2" t="str">
+        <v>NewLocation4</v>
+      </c>
+      <c r="N2" t="str">
+        <v>Written Down Value</v>
+      </c>
+      <c r="O2" t="str">
+        <v>GreatestDetective</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>6</v>
+      </c>
+      <c r="B3" t="str">
+        <v>ISBN 987-897231232</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45058.000185185185</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Good</v>
+      </c>
+      <c r="E3">
+        <v>10000</v>
+      </c>
+      <c r="F3">
+        <v>1000</v>
+      </c>
+      <c r="G3">
         <v>10</v>
       </c>
-      <c r="I2" t="str">
-        <v>010200000160</v>
-      </c>
-      <c r="J2" t="str">
-        <v>This is a test asset</v>
-      </c>
-      <c r="K2" t="str">
-        <v>2024-02-27</v>
-      </c>
-      <c r="L2">
+      <c r="H3" t="str">
+        <v>AUA1000</v>
+      </c>
+      <c r="I3" t="str">
+        <v>This would have been an epic description but nah</v>
+      </c>
+      <c r="J3" s="1">
+        <v>45150.000185185185</v>
+      </c>
+      <c r="K3" t="b">
         <v>0</v>
       </c>
-      <c r="M2" t="str">
-        <v>TestLocation</v>
-      </c>
-      <c r="N2" t="str">
-        <v>all</v>
-      </c>
-      <c r="O2" t="str">
-        <v>all</v>
+      <c r="L3" t="str">
+        <v>NewCategory</v>
+      </c>
+      <c r="M3" t="str">
+        <v>NewLocation4</v>
+      </c>
+      <c r="N3" t="str">
+        <v>Written Down Value</v>
+      </c>
+      <c r="O3" t="str">
+        <v>GreatestDetective</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>9</v>
+      </c>
+      <c r="B4" t="str">
+        <v>ISBN 987-897231232</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45058.000185185185</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Good</v>
+      </c>
+      <c r="E4">
+        <v>10000</v>
+      </c>
+      <c r="F4">
+        <v>1000</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4" t="str">
+        <v>AUA1003</v>
+      </c>
+      <c r="I4" t="str">
+        <v>This would have been an epic description but nah</v>
+      </c>
+      <c r="J4" s="1">
+        <v>45152.000185185185</v>
+      </c>
+      <c r="K4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" t="str">
+        <v>NewCategory</v>
+      </c>
+      <c r="M4" t="str">
+        <v>NewLocation4</v>
+      </c>
+      <c r="N4" t="str">
+        <v>Written Down Value</v>
+      </c>
+      <c r="O4" t="str">
+        <v>GreatestDetective</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5" t="str">
+        <v>ISBN 987-897231232</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45058.000185185185</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Good</v>
+      </c>
+      <c r="E5">
+        <v>10000</v>
+      </c>
+      <c r="F5">
+        <v>1000</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5" t="str">
+        <v>AUA1004</v>
+      </c>
+      <c r="I5" t="str">
+        <v>This would have been an epic description but nah</v>
+      </c>
+      <c r="J5" s="1">
+        <v>45152.000185185185</v>
+      </c>
+      <c r="K5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" t="str">
+        <v>NewCategory</v>
+      </c>
+      <c r="M5" t="str">
+        <v>NewLocation4</v>
+      </c>
+      <c r="N5" t="str">
+        <v>Written Down Value</v>
+      </c>
+      <c r="O5" t="str">
+        <v>GreatestDetective</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>11</v>
+      </c>
+      <c r="B6" t="str">
+        <v>ISBN 987-897231232</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45058.000185185185</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Good</v>
+      </c>
+      <c r="E6">
+        <v>10000</v>
+      </c>
+      <c r="F6">
+        <v>1000</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6" t="str">
+        <v>AUA1004</v>
+      </c>
+      <c r="I6" t="str">
+        <v>This would have been an epic description but nah</v>
+      </c>
+      <c r="J6" s="1">
+        <v>45155.000185185185</v>
+      </c>
+      <c r="K6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" t="str">
+        <v>NewCategory</v>
+      </c>
+      <c r="M6" t="str">
+        <v>NewLocation4</v>
+      </c>
+      <c r="N6" t="str">
+        <v>Written Down Value</v>
+      </c>
+      <c r="O6" t="str">
+        <v>GreatestDetective</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="str">
+        <v>ISBN 987-897231232</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45058.000185185185</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Good</v>
+      </c>
+      <c r="E7">
+        <v>10000</v>
+      </c>
+      <c r="F7">
+        <v>1000</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7" t="str">
+        <v>AUA1000</v>
+      </c>
+      <c r="I7" t="str">
+        <v>This would have been an epic description but nah</v>
+      </c>
+      <c r="J7" s="1">
+        <v>45150.000185185185</v>
+      </c>
+      <c r="K7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" t="str">
+        <v>NewCategory</v>
+      </c>
+      <c r="M7" t="str">
+        <v>NewLocation4</v>
+      </c>
+      <c r="N7" t="str">
+        <v>Written Down Value</v>
+      </c>
+      <c r="O7" t="str">
+        <v>GreatestDetective</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>